<commit_message>
Update tariff regional aggregation based on CEPII, Guimbard (2012)
</commit_message>
<xml_diff>
--- a/tables/message_scenarios.xlsx
+++ b/tables/message_scenarios.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE94E0-7FCC-4AB6-B461-E0235A383101}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ABDF78-3918-4336-A2C0-743DF9576F6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DEABEAE1-75A3-47F1-AD0F-73C499BC0073}"/>
   </bookViews>
   <sheets>
     <sheet name="unformatted" sheetId="1" r:id="rId1"/>
+    <sheet name="Formatted" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Scenario</t>
   </si>
@@ -69,12 +71,6 @@
     <t>Low tariff</t>
   </si>
   <si>
-    <t>Distance and tariff-differentiated variable costs, tariffs rates set to 10% of historic mean for region (for model years)</t>
-  </si>
-  <si>
-    <t>Distance and tariff-differentiated variable costs, tariffs rates set to two times historic mean for the region (for model years)</t>
-  </si>
-  <si>
     <t>Scenario name</t>
   </si>
   <si>
@@ -97,13 +93,100 @@
   </si>
   <si>
     <t>Sanctions between North America and Centrally Planned Asia</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>oil_exp_cpa</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>oil_exp_nam</t>
+  </si>
+  <si>
+    <t>oil_exp_pao</t>
+  </si>
+  <si>
+    <t>oil_exp_pas</t>
+  </si>
+  <si>
+    <t>oil_exp_sas</t>
+  </si>
+  <si>
+    <t>oil_exp_weu</t>
+  </si>
+  <si>
+    <t>oil_exp</t>
+  </si>
+  <si>
+    <t>Sanctions between Centrally Planned Asia and Pacific-Oceania</t>
+  </si>
+  <si>
+    <t>CPA_PAO_sanction</t>
+  </si>
+  <si>
+    <t>NAM_MEA_sanction</t>
+  </si>
+  <si>
+    <t>Sanctions between North America and Middle East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total systems cost </t>
+  </si>
+  <si>
+    <t>Apply CO2 price, with baseline tariffs</t>
+  </si>
+  <si>
+    <t>Apply CO2 price, with high tariff scenario</t>
+  </si>
+  <si>
+    <t>Apply CO2 price, with low tariff scenario</t>
+  </si>
+  <si>
+    <t>CO2_tax_baseline</t>
+  </si>
+  <si>
+    <t>CO2_tax_tariff_high</t>
+  </si>
+  <si>
+    <t>CO2_tax_tariff_low</t>
+  </si>
+  <si>
+    <t>Add $30/tCO2 tax on emissions, allowing increase of 5% per year from 2020, cap at $100/tCO2</t>
+  </si>
+  <si>
+    <t>Distance and tariff-differentiated variable costs, tariffs rates set to two times historic region median</t>
+  </si>
+  <si>
+    <t>Distance and tariff-differentiated variable costs, tariffs rates set to 0% of historical region median</t>
+  </si>
+  <si>
+    <t>NAM_MEA_sanction_onlydirect</t>
+  </si>
+  <si>
+    <t>Sanction between NAM and MEA, no indirect effects</t>
+  </si>
+  <si>
+    <t>Make trade between NAM and MEA prohibitively expensive in 2020-2025</t>
+  </si>
+  <si>
+    <t>Make trade between NAM and MEA prohibitively expensive, increase embodied cost by 20% for other regions' trade with NAM (MEA) if counterfactual has them trade with CPA (MEA)</t>
+  </si>
+  <si>
+    <t>Make trade between CPA and PAO prohibitively expensive, increase embodied cost by 20% for other regions' trade with CPA (PAO) if counterfactual has them trade with PAO (CPA)</t>
+  </si>
+  <si>
+    <t>Make trade between NAM and CPA prohibitively expensive, increase embodied cost by 20% for other regions' trade with NAM (CPA) if counterfactual has them trade with CPA (NAM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,16 +202,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -136,17 +264,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -463,15 +722,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86284D5B-991C-4D79-8417-C9963EA5CC7C}">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -481,10 +741,10 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -498,98 +758,643 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2516900.6800000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2515551.7000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="28">
+        <v>15</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="28">
+        <v>2525919.98</v>
+      </c>
+      <c r="F5" s="28">
+        <f>(E5-$E$5)/$E$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
+      <c r="B6" s="28">
+        <v>15</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="28">
+        <v>2556370.6800000002</v>
+      </c>
+      <c r="F6" s="28">
+        <f>(E6-$E$5)/$E$5</f>
+        <v>1.2055290841002883E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="26">
+        <v>9</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="26">
+        <v>2515551.7000000002</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" ref="F6:F13" si="0">(E7-$E$5)/$E$5</f>
+        <v>-4.1047539439471063E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="21">
+        <v>9</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="19">
+        <v>7</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="26">
+        <v>8</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="26">
+        <v>10591302.869999999</v>
+      </c>
+      <c r="F10" s="26">
+        <f t="shared" si="0"/>
+        <v>3.1930476633705549</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="25">
+        <v>25</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="21">
+        <v>9</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="21">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="23">
+        <v>6</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="28">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>2516900.6800000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>2523993.21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>2525372.0499999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>2526662.96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
+      <c r="C14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="26">
+        <v>10591087.439999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8823AD7C-1F93-412C-A85F-85B836AA1EE4}">
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="15"/>
+    <col min="3" max="3" width="71" style="15" customWidth="1"/>
+    <col min="4" max="4" width="95" style="16" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="str">
+        <f>unformatted!A3</f>
+        <v>baseline_global_schema</v>
+      </c>
+      <c r="B3" s="14">
+        <f>unformatted!B3</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="18" t="str">
+        <f>unformatted!C3</f>
+        <v>Baseline (global schema)</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f>unformatted!D3</f>
+        <v>Global schema, no variable costs or shipping technologies</v>
+      </c>
+      <c r="E3" s="8">
+        <f>unformatted!E3</f>
+        <v>2516900.6800000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="str">
+        <f>unformatted!A4</f>
+        <v>baseline_no_tariff</v>
+      </c>
+      <c r="B4" s="14">
+        <f>unformatted!B4</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="18" t="str">
+        <f>unformatted!C4</f>
+        <v>Baseline, distance only</v>
+      </c>
+      <c r="D4" s="17" t="str">
+        <f>unformatted!D4</f>
+        <v>Baseline distance-differentiated variable costs</v>
+      </c>
+      <c r="E4" s="8">
+        <f>unformatted!E4</f>
+        <v>2515551.7000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="str">
+        <f>unformatted!A5</f>
+        <v>baseline</v>
+      </c>
+      <c r="B5" s="14">
+        <f>unformatted!B5</f>
+        <v>15</v>
+      </c>
+      <c r="C5" s="18" t="str">
+        <f>unformatted!C5</f>
+        <v>Baseline, distance and tariff</v>
+      </c>
+      <c r="D5" s="17" t="str">
+        <f>unformatted!D5</f>
+        <v>Baseline distance and tariff-differentiated variable costs</v>
+      </c>
+      <c r="E5" s="8">
+        <f>unformatted!E5</f>
+        <v>2525919.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="str">
+        <f>unformatted!A6</f>
+        <v>tariff_high</v>
+      </c>
+      <c r="B6" s="14">
+        <f>unformatted!B6</f>
+        <v>15</v>
+      </c>
+      <c r="C6" s="18" t="str">
+        <f>unformatted!C6</f>
+        <v>High tariff</v>
+      </c>
+      <c r="D6" s="17" t="str">
+        <f>unformatted!D6</f>
+        <v>Distance and tariff-differentiated variable costs, tariffs rates set to two times historic region median</v>
+      </c>
+      <c r="E6" s="8">
+        <f>unformatted!E6</f>
+        <v>2556370.6800000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="str">
+        <f>unformatted!A7</f>
+        <v>tariff_low</v>
+      </c>
+      <c r="B7" s="14">
+        <f>unformatted!B7</f>
+        <v>9</v>
+      </c>
+      <c r="C7" s="18" t="str">
+        <f>unformatted!C7</f>
+        <v>Low tariff</v>
+      </c>
+      <c r="D7" s="17" t="str">
+        <f>unformatted!D7</f>
+        <v>Distance and tariff-differentiated variable costs, tariffs rates set to 0% of historical region median</v>
+      </c>
+      <c r="E7" s="8">
+        <f>unformatted!E7</f>
+        <v>2515551.7000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="str">
+        <f>unformatted!A8</f>
+        <v>NAM_CPA_sanction</v>
+      </c>
+      <c r="B8" s="14">
+        <f>unformatted!B8</f>
+        <v>9</v>
+      </c>
+      <c r="C8" s="18" t="str">
+        <f>unformatted!C8</f>
+        <v>Sanctions between North America and Centrally Planned Asia</v>
+      </c>
+      <c r="D8" s="17" t="str">
+        <f>unformatted!D8</f>
+        <v>Make trade between NAM and CPA prohibitively expensive, increase embodied cost by 20% for other regions' trade with NAM (CPA) if counterfactual has them trade with CPA (NAM)</v>
+      </c>
+      <c r="E8" s="8">
+        <f>unformatted!E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="str">
+        <f>unformatted!A9</f>
+        <v>CPA_PAO_sanction</v>
+      </c>
+      <c r="B9" s="14">
+        <f>unformatted!B9</f>
+        <v>7</v>
+      </c>
+      <c r="C9" s="18" t="str">
+        <f>unformatted!C9</f>
+        <v>Sanctions between Centrally Planned Asia and Pacific-Oceania</v>
+      </c>
+      <c r="D9" s="17" t="str">
+        <f>unformatted!D9</f>
+        <v>Make trade between CPA and PAO prohibitively expensive, increase embodied cost by 20% for other regions' trade with CPA (PAO) if counterfactual has them trade with PAO (CPA)</v>
+      </c>
+      <c r="E9" s="8">
+        <f>unformatted!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="str">
+        <f>unformatted!A10</f>
+        <v>NAM_MEA_sanction</v>
+      </c>
+      <c r="B10" s="14">
+        <f>unformatted!B10</f>
+        <v>8</v>
+      </c>
+      <c r="C10" s="18" t="str">
+        <f>unformatted!C10</f>
+        <v>Sanctions between North America and Middle East</v>
+      </c>
+      <c r="D10" s="17" t="str">
+        <f>unformatted!D10</f>
+        <v>Make trade between NAM and MEA prohibitively expensive, increase embodied cost by 20% for other regions' trade with NAM (MEA) if counterfactual has them trade with CPA (MEA)</v>
+      </c>
+      <c r="E10" s="8">
+        <f>unformatted!E10</f>
+        <v>10591302.869999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="str">
+        <f>unformatted!A11</f>
+        <v>CO2_tax_baseline</v>
+      </c>
+      <c r="B11" s="14">
+        <f>unformatted!B11</f>
+        <v>25</v>
+      </c>
+      <c r="C11" s="18" t="str">
+        <f>unformatted!C11</f>
+        <v>Apply CO2 price, with baseline tariffs</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <f>unformatted!D11</f>
+        <v>Add $30/tCO2 tax on emissions, allowing increase of 5% per year from 2020, cap at $100/tCO2</v>
+      </c>
+      <c r="E11" s="8">
+        <f>unformatted!E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="str">
+        <f>unformatted!A12</f>
+        <v>CO2_tax_tariff_high</v>
+      </c>
+      <c r="B12" s="14">
+        <f>unformatted!B12</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="str">
+        <f>unformatted!C12</f>
+        <v>Apply CO2 price, with high tariff scenario</v>
+      </c>
+      <c r="D12" s="17" t="str">
+        <f>unformatted!D12</f>
+        <v>Add $30/tCO2 tax on emissions, allowing increase of 5% per year from 2020, cap at $100/tCO2</v>
+      </c>
+      <c r="E12" s="8">
+        <f>unformatted!E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="str">
+        <f>unformatted!A13</f>
+        <v>CO2_tax_tariff_low</v>
+      </c>
+      <c r="B13" s="14">
+        <f>unformatted!B13</f>
+        <v>6</v>
+      </c>
+      <c r="C13" s="18" t="str">
+        <f>unformatted!C13</f>
+        <v>Apply CO2 price, with low tariff scenario</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <f>unformatted!D13</f>
+        <v>Add $30/tCO2 tax on emissions, allowing increase of 5% per year from 2020, cap at $100/tCO2</v>
+      </c>
+      <c r="E13" s="8">
+        <f>unformatted!E13</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7F9641-E7FB-4025-B4A1-8A24448BCDF4}">
+  <dimension ref="A14:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>353.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>362.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>525.29999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>378.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>596.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>2764.9</v>
+      </c>
+      <c r="E21">
+        <f>SUM(D15:D20)</f>
+        <v>2764.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>